<commit_message>
Spatial parameters for all cases
</commit_message>
<xml_diff>
--- a/spatial_parameters all cases.xlsx
+++ b/spatial_parameters all cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdallahy\Documents\GitHub\melbourne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CE5465-4014-4758-9BBF-8A3621469E7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A108793-1486-431C-83D3-62FC3DBD435C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -101,14 +101,86 @@
   </si>
   <si>
     <t>Free Flow</t>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (entry pressure) (pa)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lamda</t>
+  </si>
+  <si>
+    <r>
+      <t>swr (for p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>swr (for relative permeability)</t>
+  </si>
+  <si>
+    <t>snc (critical saturation)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,8 +208,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,14 +239,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>433845</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>78230</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -183,8 +261,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="0" y="4610100"/>
-          <a:ext cx="9577845" cy="4231130"/>
+          <a:off x="0" y="4486275"/>
+          <a:ext cx="9267825" cy="3476625"/>
           <a:chOff x="0" y="5512575"/>
           <a:chExt cx="9577845" cy="4231130"/>
         </a:xfrm>
@@ -291,6 +369,60 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>180974</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>356346</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B2745F4-D0D9-459A-B1A8-713661CA70B9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -556,17 +688,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9.8692299999999996E-15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="1">
+        <v>500000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.4547299999999993E-9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.4994860559999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4.20331E-9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3.62620904</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.11990000000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.9787800000000001E-9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="D5" s="1">
+        <v>363</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.1196</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.09548E-9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D6" s="1">
+        <v>657.27</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.6960533330000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.1167</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.6681500000000001E-10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1442.07</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.6909909089999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.1356</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.66469E-11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6058.88</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.31968000000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.3424600000000003E-11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6058.88</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.31968000000000002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.1843099999999999E-8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.DSMT4" shapeId="1025" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" altText="" r:id="rId5">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>180975</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>352425</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.DSMT4" shapeId="1025" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
 

</xml_diff>